<commit_message>
Completed zip --> timestepped process
</commit_message>
<xml_diff>
--- a/Sub List.xlsx
+++ b/Sub List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="21210" yWindow="-15" windowWidth="7605" windowHeight="13455" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="22020" windowHeight="12990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2643" uniqueCount="1371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2646" uniqueCount="1374">
   <si>
     <t>Index</t>
   </si>
@@ -4132,6 +4132,15 @@
   </si>
   <si>
     <t>Num Used</t>
+  </si>
+  <si>
+    <t>^Too east</t>
+  </si>
+  <si>
+    <t>SB:</t>
+  </si>
+  <si>
+    <t>Mono:</t>
   </si>
 </sst>
 </file>
@@ -4612,7 +4621,7 @@
   <dimension ref="A1:N4103"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H1287" sqref="H1287"/>
+      <selection activeCell="B1306" sqref="B1306"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4724,7 +4733,7 @@
         <v>1357</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1001</v>
       </c>
@@ -4877,7 +4886,7 @@
         <v>0.65691655152124695</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1268</v>
       </c>
@@ -5064,7 +5073,7 @@
         <v>0.76200428122421415</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>975</v>
       </c>
@@ -5099,7 +5108,7 @@
         <v>0.3535892056968914</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1156</v>
       </c>
@@ -5438,7 +5447,7 @@
         <v>0.958751079661189</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>731</v>
       </c>
@@ -5511,7 +5520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>737</v>
       </c>
@@ -5892,7 +5901,7 @@
         <v>0.49223660224524257</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1196</v>
       </c>
@@ -5969,7 +5978,7 @@
         <v>0.38740999541230609</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>854</v>
       </c>
@@ -6688,7 +6697,7 @@
         <v>0.9282871906253809</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>955</v>
       </c>
@@ -6769,7 +6778,7 @@
         <v>0.90121427107719476</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>895</v>
       </c>
@@ -7032,7 +7041,7 @@
         <v>0.67431180524220302</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1157</v>
       </c>
@@ -7105,7 +7114,7 @@
         <v>0.26658482690904717</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1240</v>
       </c>
@@ -7143,7 +7152,7 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>1154</v>
       </c>
@@ -7216,7 +7225,7 @@
         <v>0.96668468504161298</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1212</v>
       </c>
@@ -7327,7 +7336,7 @@
         <v>0.97115071648534901</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1087</v>
       </c>
@@ -7970,7 +7979,7 @@
         <v>0.70970115717126347</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>716</v>
       </c>
@@ -8309,7 +8318,7 @@
         <v>0.45046808468743066</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>964</v>
       </c>
@@ -8428,7 +8437,7 @@
         <v>0.64433699008797352</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>190</v>
       </c>
@@ -8474,7 +8483,7 @@
         <v>212.53596872372825</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1222</v>
       </c>
@@ -8509,7 +8518,7 @@
         <v>0.93877789034996961</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>319</v>
       </c>
@@ -8699,7 +8708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>366</v>
       </c>
@@ -8737,7 +8746,7 @@
         <v>0.5107549467039213</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>883</v>
       </c>
@@ -8776,7 +8785,7 @@
         <v>0.33566011228104536</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>715</v>
       </c>
@@ -8815,7 +8824,7 @@
         <v>0.74985455933026646</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>654</v>
       </c>
@@ -8853,7 +8862,7 @@
         <v>0.45718054344073755</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>570</v>
       </c>
@@ -8891,7 +8900,7 @@
         <v>0.39165968357074316</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>525</v>
       </c>
@@ -8929,7 +8938,7 @@
         <v>0.10223747963730236</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>440</v>
       </c>
@@ -8967,7 +8976,7 @@
         <v>0.17489361388202768</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>575</v>
       </c>
@@ -9081,7 +9090,7 @@
         <v>0.98989287866521025</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>332</v>
       </c>
@@ -9122,7 +9131,7 @@
         <v>1349</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>445</v>
       </c>
@@ -9160,7 +9169,7 @@
         <v>0.41726574646548847</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>393</v>
       </c>
@@ -9198,7 +9207,7 @@
         <v>0.94478965580835117</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>322</v>
       </c>
@@ -9243,7 +9252,7 @@
         <v>323.5526418891543</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>488</v>
       </c>
@@ -9323,7 +9332,7 @@
         <v>0.66622525241051644</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>483</v>
       </c>
@@ -9364,7 +9373,7 @@
         <v>1350</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>399</v>
       </c>
@@ -9520,7 +9529,7 @@
         <v>9.6943138638406021E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>646</v>
       </c>
@@ -9600,7 +9609,7 @@
         <v>0.36105564854607847</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>446</v>
       </c>
@@ -9642,7 +9651,7 @@
         <v>0.58158967526776895</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>198</v>
       </c>
@@ -9684,7 +9693,7 @@
         <v>6.5600768072879789E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>638</v>
       </c>
@@ -9722,7 +9731,7 @@
         <v>0.93534484064709156</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>523</v>
       </c>
@@ -9802,7 +9811,7 @@
         <v>9.3962325611856995E-3</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>657</v>
       </c>
@@ -9958,7 +9967,7 @@
         <v>0.75586923087248692</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>204</v>
       </c>
@@ -9996,7 +10005,7 @@
         <v>0.97835733917957313</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>666</v>
       </c>
@@ -10042,7 +10051,7 @@
         <v>318.00593448724413</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>261</v>
       </c>
@@ -10083,7 +10092,7 @@
         <v>1351</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>520</v>
       </c>
@@ -10125,7 +10134,7 @@
         <v>0.45383470950277427</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>542</v>
       </c>
@@ -10167,7 +10176,7 @@
         <v>0.12707592332041445</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>247</v>
       </c>
@@ -10365,7 +10374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>489</v>
       </c>
@@ -10483,7 +10492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>572</v>
       </c>
@@ -10525,7 +10534,7 @@
         <v>0.48910912150370323</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>202</v>
       </c>
@@ -10605,7 +10614,7 @@
         <v>0.27532186351774912</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>169</v>
       </c>
@@ -10643,7 +10652,7 @@
         <v>0.82847461413399925</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>218</v>
       </c>
@@ -10689,7 +10698,7 @@
         <v>266.40285253810663</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>151</v>
       </c>
@@ -10735,7 +10744,7 @@
         <v>297.04196512069518</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>655</v>
       </c>
@@ -10773,7 +10782,7 @@
         <v>0.98856340855116875</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>687</v>
       </c>
@@ -10819,7 +10828,7 @@
         <v>289.26723431986596</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>499</v>
       </c>
@@ -10865,7 +10874,7 @@
         <v>126.67958776652461</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>581</v>
       </c>
@@ -10907,7 +10916,7 @@
         <v>0.11859828357386075</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>425</v>
       </c>
@@ -11059,7 +11068,7 @@
         <v>0.95161224968016755</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>398</v>
       </c>
@@ -11097,7 +11106,7 @@
         <v>0.56635828171007485</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>656</v>
       </c>
@@ -11215,7 +11224,7 @@
         <v>4.9821913579614477E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>534</v>
       </c>
@@ -11257,7 +11266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>214</v>
       </c>
@@ -11333,7 +11342,7 @@
         <v>0.99010736344655015</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>278</v>
       </c>
@@ -11375,7 +11384,7 @@
         <v>0.23440662160411466</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>403</v>
       </c>
@@ -11417,7 +11426,7 @@
         <v>0.11027401918214746</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>660</v>
       </c>
@@ -11455,7 +11464,7 @@
         <v>0.99678029238320864</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>437</v>
       </c>
@@ -11501,7 +11510,7 @@
         <v>453.60868689804738</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>616</v>
       </c>
@@ -11539,7 +11548,7 @@
         <v>0.95018872307682944</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>669</v>
       </c>
@@ -11581,7 +11590,7 @@
         <v>0.20322129280810852</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>529</v>
       </c>
@@ -11623,7 +11632,7 @@
         <v>0.47085886946758215</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>396</v>
       </c>
@@ -11703,7 +11712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>630</v>
       </c>
@@ -11783,7 +11792,7 @@
         <v>0.97248793172738035</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>297</v>
       </c>
@@ -11825,7 +11834,7 @@
         <v>9.0318978154793686E-3</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>605</v>
       </c>
@@ -11863,7 +11872,7 @@
         <v>0.90486756630724574</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>183</v>
       </c>
@@ -11989,7 +11998,7 @@
         <v>0.40498937718600891</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>469</v>
       </c>
@@ -12031,7 +12040,7 @@
         <v>0.21422209410030579</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>290</v>
       </c>
@@ -12115,7 +12124,7 @@
         <v>7.4082549751871305E-5</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>447</v>
       </c>
@@ -12157,7 +12166,7 @@
         <v>5.4734128268043789E-2</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>634</v>
       </c>
@@ -12195,7 +12204,7 @@
         <v>0.94616182535888682</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>633</v>
       </c>
@@ -12241,7 +12250,7 @@
         <v>101.97700061598812</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>530</v>
       </c>
@@ -12325,7 +12334,7 @@
         <v>0.77244279816747163</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>321</v>
       </c>
@@ -12363,7 +12372,7 @@
         <v>0.93615383675297381</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>159</v>
       </c>
@@ -12401,7 +12410,7 @@
         <v>0.93511512219083404</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>484</v>
       </c>
@@ -12477,7 +12486,7 @@
         <v>0.73688876321163532</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>560</v>
       </c>
@@ -12519,7 +12528,7 @@
         <v>0.33200511900535018</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>392</v>
       </c>
@@ -12557,7 +12566,7 @@
         <v>0.9210381070357655</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>420</v>
       </c>
@@ -12603,7 +12612,7 @@
         <v>91.085416559454373</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>579</v>
       </c>
@@ -12645,7 +12654,7 @@
         <v>0.32705230827822079</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>229</v>
       </c>
@@ -12683,7 +12692,7 @@
         <v>0.94673838072385019</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>205</v>
       </c>
@@ -12725,7 +12734,7 @@
         <v>2.0350979190625014E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>624</v>
       </c>
@@ -12767,7 +12776,7 @@
         <v>0.17321577158114571</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>593</v>
       </c>
@@ -12809,7 +12818,7 @@
         <v>5.060045531014001E-3</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>651</v>
       </c>
@@ -12851,7 +12860,7 @@
         <v>0.45321998942624464</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>272</v>
       </c>
@@ -12931,7 +12940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>639</v>
       </c>
@@ -13045,7 +13054,7 @@
         <v>0.76022371493330065</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>407</v>
       </c>
@@ -13083,7 +13092,7 @@
         <v>0.78465005547364342</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>582</v>
       </c>
@@ -13167,7 +13176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>471</v>
       </c>
@@ -13209,7 +13218,7 @@
         <v>0.26660729958438995</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>336</v>
       </c>
@@ -13247,7 +13256,7 @@
         <v>0.79129953630068961</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>466</v>
       </c>
@@ -13285,7 +13294,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>573</v>
       </c>
@@ -13403,7 +13412,7 @@
         <v>0.38133235335903615</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>577</v>
       </c>
@@ -13445,7 +13454,7 @@
         <v>0.83097342342695657</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>486</v>
       </c>
@@ -13563,7 +13572,7 @@
         <v>8.959693833092823E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>215</v>
       </c>
@@ -13601,7 +13610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>423</v>
       </c>
@@ -13643,7 +13652,7 @@
         <v>0.84230322411504843</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>456</v>
       </c>
@@ -13689,7 +13698,7 @@
         <v>410.28507775361749</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>479</v>
       </c>
@@ -13735,7 +13744,7 @@
         <v>93.680870656034486</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>584</v>
       </c>
@@ -13777,7 +13786,7 @@
         <v>0.82063009728400649</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>528</v>
       </c>
@@ -13819,7 +13828,7 @@
         <v>0.75069330095833253</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>621</v>
       </c>
@@ -13861,7 +13870,7 @@
         <v>0.77664702236883232</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>567</v>
       </c>
@@ -13941,7 +13950,7 @@
         <v>1.6603851611999404E-3</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>330</v>
       </c>
@@ -14101,7 +14110,7 @@
         <v>185.57022009708422</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>603</v>
       </c>
@@ -14253,7 +14262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>270</v>
       </c>
@@ -14291,7 +14300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>234</v>
       </c>
@@ -14333,7 +14342,7 @@
         <v>0.69201347162423266</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>421</v>
       </c>
@@ -14371,7 +14380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>130</v>
       </c>
@@ -14485,7 +14494,7 @@
         <v>0.91894269219653313</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>545</v>
       </c>
@@ -14523,7 +14532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>148</v>
       </c>
@@ -14717,7 +14726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>454</v>
       </c>
@@ -14759,7 +14768,7 @@
         <v>0.6810083993345023</v>
       </c>
     </row>
-    <row r="261" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>493</v>
       </c>
@@ -14911,7 +14920,7 @@
         <v>0.99206034440041024</v>
       </c>
     </row>
-    <row r="265" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>426</v>
       </c>
@@ -14987,7 +14996,7 @@
         <v>0.64448753301272255</v>
       </c>
     </row>
-    <row r="267" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>442</v>
       </c>
@@ -15105,7 +15114,7 @@
         <v>0.23228630165496938</v>
       </c>
     </row>
-    <row r="270" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>415</v>
       </c>
@@ -15223,7 +15232,7 @@
         <v>0.57865631441625243</v>
       </c>
     </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>505</v>
       </c>
@@ -15269,7 +15278,7 @@
         <v>42.069289413710884</v>
       </c>
     </row>
-    <row r="274" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>269</v>
       </c>
@@ -15311,7 +15320,7 @@
         <v>0.65135591860508979</v>
       </c>
     </row>
-    <row r="275" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>230</v>
       </c>
@@ -15349,7 +15358,7 @@
         <v>0.33368940284046311</v>
       </c>
     </row>
-    <row r="276" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>360</v>
       </c>
@@ -15395,7 +15404,7 @@
         <v>49.177227865707977</v>
       </c>
     </row>
-    <row r="277" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>557</v>
       </c>
@@ -15437,7 +15446,7 @@
         <v>0.76945274524196083</v>
       </c>
     </row>
-    <row r="278" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>641</v>
       </c>
@@ -15513,7 +15522,7 @@
         <v>1.1877713695935261E-2</v>
       </c>
     </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>693</v>
       </c>
@@ -15593,7 +15602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>380</v>
       </c>
@@ -15635,7 +15644,7 @@
         <v>0.66377013174099653</v>
       </c>
     </row>
-    <row r="283" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>451</v>
       </c>
@@ -15681,7 +15690,7 @@
         <v>46.920702154308927</v>
       </c>
     </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>419</v>
       </c>
@@ -15879,7 +15888,7 @@
         <v>4.7395285507344662E-2</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>672</v>
       </c>
@@ -15917,7 +15926,7 @@
         <v>2.2857201917487201E-2</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>165</v>
       </c>
@@ -16035,7 +16044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>441</v>
       </c>
@@ -16077,7 +16086,7 @@
         <v>0.61651095724685845</v>
       </c>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>351</v>
       </c>
@@ -16119,7 +16128,7 @@
         <v>0.79625174936385124</v>
       </c>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>246</v>
       </c>
@@ -16313,7 +16322,7 @@
         <v>0.92360168581028834</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>475</v>
       </c>
@@ -16354,7 +16363,7 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>674</v>
       </c>
@@ -16434,7 +16443,7 @@
         <v>3.0702232480423385E-2</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>676</v>
       </c>
@@ -16472,7 +16481,7 @@
         <v>0.99458559198963947</v>
       </c>
     </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>370</v>
       </c>
@@ -16632,7 +16641,7 @@
         <v>0.85923812402634792</v>
       </c>
     </row>
-    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>111</v>
       </c>
@@ -16712,7 +16721,7 @@
         <v>0.28904952018597707</v>
       </c>
     </row>
-    <row r="310" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>461</v>
       </c>
@@ -16750,7 +16759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>591</v>
       </c>
@@ -16791,7 +16800,7 @@
         <v>1365</v>
       </c>
     </row>
-    <row r="312" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>558</v>
       </c>
@@ -16837,7 +16846,7 @@
         <v>133.74396955688027</v>
       </c>
     </row>
-    <row r="313" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>324</v>
       </c>
@@ -16917,7 +16926,7 @@
         <v>0.98201367205502932</v>
       </c>
     </row>
-    <row r="315" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>533</v>
       </c>
@@ -16959,7 +16968,7 @@
         <v>0.15029175469751097</v>
       </c>
     </row>
-    <row r="316" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>353</v>
       </c>
@@ -17000,7 +17009,7 @@
         <v>1366</v>
       </c>
     </row>
-    <row r="317" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>300</v>
       </c>
@@ -17042,7 +17051,7 @@
         <v>0.41271075460419326</v>
       </c>
     </row>
-    <row r="318" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>251</v>
       </c>
@@ -17160,7 +17169,7 @@
         <v>0.93100952619756494</v>
       </c>
     </row>
-    <row r="321" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>219</v>
       </c>
@@ -17202,7 +17211,7 @@
         <v>0.63284608186914959</v>
       </c>
     </row>
-    <row r="322" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>196</v>
       </c>
@@ -17244,7 +17253,7 @@
         <v>0.41919582989813142</v>
       </c>
     </row>
-    <row r="323" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>185</v>
       </c>
@@ -17328,7 +17337,7 @@
         <v>0.49520960178570311</v>
       </c>
     </row>
-    <row r="325" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>390</v>
       </c>
@@ -17370,7 +17379,7 @@
         <v>0.36578605986989543</v>
       </c>
     </row>
-    <row r="326" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>289</v>
       </c>
@@ -17450,7 +17459,7 @@
         <v>0.56771660142781688</v>
       </c>
     </row>
-    <row r="328" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>608</v>
       </c>
@@ -17488,7 +17497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>417</v>
       </c>
@@ -17572,7 +17581,7 @@
         <v>0.85173853560646373</v>
       </c>
     </row>
-    <row r="331" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>172</v>
       </c>
@@ -17652,7 +17661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="333" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>539</v>
       </c>
@@ -17694,7 +17703,7 @@
         <v>0.45704602357169988</v>
       </c>
     </row>
-    <row r="334" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>585</v>
       </c>
@@ -17777,7 +17786,7 @@
         <v>5.1310443623162519E-2</v>
       </c>
     </row>
-    <row r="336" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>239</v>
       </c>
@@ -17891,7 +17900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="339" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>611</v>
       </c>
@@ -17933,7 +17942,7 @@
         <v>0.46805373268405698</v>
       </c>
     </row>
-    <row r="340" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>233</v>
       </c>
@@ -17975,7 +17984,7 @@
         <v>0.70433555212921473</v>
       </c>
     </row>
-    <row r="341" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>106</v>
       </c>
@@ -18169,7 +18178,7 @@
         <v>9.0437335539913857E-3</v>
       </c>
     </row>
-    <row r="346" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>408</v>
       </c>
@@ -18249,7 +18258,7 @@
         <v>0.57908061979327208</v>
       </c>
     </row>
-    <row r="348" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>668</v>
       </c>
@@ -18290,7 +18299,7 @@
         <v>1368</v>
       </c>
     </row>
-    <row r="349" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>318</v>
       </c>
@@ -18332,7 +18341,7 @@
         <v>4.4130716076418927E-2</v>
       </c>
     </row>
-    <row r="350" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>430</v>
       </c>
@@ -18370,7 +18379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>206</v>
       </c>
@@ -18484,7 +18493,7 @@
         <v>0.66108182415988737</v>
       </c>
     </row>
-    <row r="354" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>631</v>
       </c>
@@ -18526,7 +18535,7 @@
         <v>0.71895788403717198</v>
       </c>
     </row>
-    <row r="355" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>400</v>
       </c>
@@ -18568,7 +18577,7 @@
         <v>0.70698505741092377</v>
       </c>
     </row>
-    <row r="356" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>158</v>
       </c>
@@ -18606,7 +18615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="357" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>620</v>
       </c>
@@ -18648,7 +18657,7 @@
         <v>0.67675578793752156</v>
       </c>
     </row>
-    <row r="358" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>594</v>
       </c>
@@ -18690,7 +18699,7 @@
         <v>0.20911318722037725</v>
       </c>
     </row>
-    <row r="359" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>546</v>
       </c>
@@ -18732,7 +18741,7 @@
         <v>0.75855881884524301</v>
       </c>
     </row>
-    <row r="360" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>327</v>
       </c>
@@ -18812,7 +18821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="362" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>113</v>
       </c>
@@ -18854,7 +18863,7 @@
         <v>0.53107962762764627</v>
       </c>
     </row>
-    <row r="363" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>306</v>
       </c>
@@ -18896,7 +18905,7 @@
         <v>0.9244381151370914</v>
       </c>
     </row>
-    <row r="364" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>109</v>
       </c>
@@ -18976,7 +18985,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>356</v>
       </c>
@@ -19056,7 +19065,7 @@
         <v>0.80382814079462983</v>
       </c>
     </row>
-    <row r="368" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>116</v>
       </c>
@@ -19098,7 +19107,7 @@
         <v>0.13324269902462413</v>
       </c>
     </row>
-    <row r="369" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>386</v>
       </c>
@@ -19144,7 +19153,7 @@
         <v>37.322212697633177</v>
       </c>
     </row>
-    <row r="370" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>604</v>
       </c>
@@ -19186,7 +19195,7 @@
         <v>0.8011984672624447</v>
       </c>
     </row>
-    <row r="371" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>337</v>
       </c>
@@ -19228,7 +19237,7 @@
         <v>0.66638548868847824</v>
       </c>
     </row>
-    <row r="372" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>613</v>
       </c>
@@ -19270,7 +19279,7 @@
         <v>0.77250758463714964</v>
       </c>
     </row>
-    <row r="373" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>462</v>
       </c>
@@ -19308,7 +19317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="374" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>536</v>
       </c>
@@ -19384,7 +19393,7 @@
         <v>9.5966478301602168E-2</v>
       </c>
     </row>
-    <row r="376" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>472</v>
       </c>
@@ -19692,7 +19701,7 @@
         <v>0.38079624976231352</v>
       </c>
     </row>
-    <row r="384" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="384" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>650</v>
       </c>
@@ -19730,7 +19739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="385" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="385" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>325</v>
       </c>
@@ -19768,7 +19777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="386" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="386" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>413</v>
       </c>
@@ -19810,7 +19819,7 @@
         <v>0.7933162175443661</v>
       </c>
     </row>
-    <row r="387" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>221</v>
       </c>
@@ -19852,7 +19861,7 @@
         <v>0.8406869547761826</v>
       </c>
     </row>
-    <row r="388" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>606</v>
       </c>
@@ -19898,7 +19907,7 @@
         <v>25.620499834033197</v>
       </c>
     </row>
-    <row r="389" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>304</v>
       </c>
@@ -19944,7 +19953,7 @@
         <v>33.998021256299985</v>
       </c>
     </row>
-    <row r="390" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>110</v>
       </c>
@@ -20024,7 +20033,7 @@
         <v>3.0193005382505747E-3</v>
       </c>
     </row>
-    <row r="392" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>433</v>
       </c>
@@ -20104,7 +20113,7 @@
         <v>0.58526397542743525</v>
       </c>
     </row>
-    <row r="394" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>201</v>
       </c>
@@ -20146,7 +20155,7 @@
         <v>0.75210198674324324</v>
       </c>
     </row>
-    <row r="395" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>609</v>
       </c>
@@ -20192,7 +20201,7 @@
         <v>17.301957445634216</v>
       </c>
     </row>
-    <row r="396" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>568</v>
       </c>
@@ -20234,7 +20243,7 @@
         <v>0.95660948051921602</v>
       </c>
     </row>
-    <row r="397" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>485</v>
       </c>
@@ -20313,7 +20322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="399" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>276</v>
       </c>
@@ -20355,7 +20364,7 @@
         <v>0.87667712815570287</v>
       </c>
     </row>
-    <row r="400" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>308</v>
       </c>
@@ -20431,7 +20440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="402" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="402" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>263</v>
       </c>
@@ -20473,7 +20482,7 @@
         <v>0.76130863908266744</v>
       </c>
     </row>
-    <row r="403" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="403" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>129</v>
       </c>
@@ -20515,7 +20524,7 @@
         <v>0.87756543439690682</v>
       </c>
     </row>
-    <row r="404" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="404" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>541</v>
       </c>
@@ -20557,7 +20566,7 @@
         <v>0.96812260643962367</v>
       </c>
     </row>
-    <row r="405" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="405" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>140</v>
       </c>
@@ -20637,7 +20646,7 @@
         <v>2.544127597851328E-2</v>
       </c>
     </row>
-    <row r="407" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>367</v>
       </c>
@@ -20675,7 +20684,7 @@
         <v>6.1627305744197235E-3</v>
       </c>
     </row>
-    <row r="408" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>627</v>
       </c>
@@ -20713,7 +20722,7 @@
         <v>9.7562098352448989E-4</v>
       </c>
     </row>
-    <row r="409" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="409" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>434</v>
       </c>
@@ -20755,7 +20764,7 @@
         <v>0.95797054740327536</v>
       </c>
     </row>
-    <row r="410" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="410" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>464</v>
       </c>
@@ -20797,7 +20806,7 @@
         <v>0.73544284509368252</v>
       </c>
     </row>
-    <row r="411" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="411" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>157</v>
       </c>
@@ -20915,7 +20924,7 @@
         <v>1.4228601198467961E-2</v>
       </c>
     </row>
-    <row r="414" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="414" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>576</v>
       </c>
@@ -20995,7 +21004,7 @@
         <v>3.4291661833125335E-3</v>
       </c>
     </row>
-    <row r="416" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="416" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>504</v>
       </c>
@@ -21037,7 +21046,7 @@
         <v>8.6612269619144783E-2</v>
       </c>
     </row>
-    <row r="417" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="417" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>352</v>
       </c>
@@ -21083,7 +21092,7 @@
         <v>41.750143727053718</v>
       </c>
     </row>
-    <row r="418" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="418" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>329</v>
       </c>
@@ -21163,7 +21172,7 @@
         <v>0.99343545731570648</v>
       </c>
     </row>
-    <row r="420" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="420" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>192</v>
       </c>
@@ -21205,7 +21214,7 @@
         <v>0.77059408151146047</v>
       </c>
     </row>
-    <row r="421" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="421" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>458</v>
       </c>
@@ -21251,7 +21260,7 @@
         <v>31.025758742132854</v>
       </c>
     </row>
-    <row r="422" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>117</v>
       </c>
@@ -21293,7 +21302,7 @@
         <v>0.85227077724497247</v>
       </c>
     </row>
-    <row r="423" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="423" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>155</v>
       </c>
@@ -21339,7 +21348,7 @@
         <v>9.4823937746651907</v>
       </c>
     </row>
-    <row r="424" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="424" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>112</v>
       </c>
@@ -21385,7 +21394,7 @@
         <v>43.413993600167757</v>
       </c>
     </row>
-    <row r="425" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="425" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>120</v>
       </c>
@@ -21427,7 +21436,7 @@
         <v>0.84736452725326883</v>
       </c>
     </row>
-    <row r="426" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>601</v>
       </c>
@@ -21507,7 +21516,7 @@
         <v>4.8490355398156472E-2</v>
       </c>
     </row>
-    <row r="428" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="428" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>382</v>
       </c>
@@ -21549,7 +21558,7 @@
         <v>0.73889789339829648</v>
       </c>
     </row>
-    <row r="429" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="429" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>429</v>
       </c>
@@ -21591,7 +21600,7 @@
         <v>0.7084676482636223</v>
       </c>
     </row>
-    <row r="430" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="430" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>299</v>
       </c>
@@ -21633,7 +21642,7 @@
         <v>0.82360694940490464</v>
       </c>
     </row>
-    <row r="431" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="431" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>443</v>
       </c>
@@ -21675,7 +21684,7 @@
         <v>0.69843986189675467</v>
       </c>
     </row>
-    <row r="432" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="432" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>625</v>
       </c>
@@ -21717,7 +21726,7 @@
         <v>0.89404403661427168</v>
       </c>
     </row>
-    <row r="433" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="433" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>200</v>
       </c>
@@ -21797,7 +21806,7 @@
         <v>0.74108420382293472</v>
       </c>
     </row>
-    <row r="435" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="435" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>626</v>
       </c>
@@ -21839,7 +21848,7 @@
         <v>0.82375894431026719</v>
       </c>
     </row>
-    <row r="436" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="436" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>359</v>
       </c>
@@ -21881,7 +21890,7 @@
         <v>0.69180842327337322</v>
       </c>
     </row>
-    <row r="437" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="437" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>487</v>
       </c>
@@ -21961,7 +21970,7 @@
         <v>0.86208935650825802</v>
       </c>
     </row>
-    <row r="439" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="439" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>160</v>
       </c>
@@ -22003,7 +22012,7 @@
         <v>0.62370256110951527</v>
       </c>
     </row>
-    <row r="440" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="440" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>138</v>
       </c>
@@ -22045,7 +22054,7 @@
         <v>0.93678505055616124</v>
       </c>
     </row>
-    <row r="441" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="441" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>383</v>
       </c>
@@ -22125,7 +22134,7 @@
         <v>0.58927384472583033</v>
       </c>
     </row>
-    <row r="443" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="443" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>551</v>
       </c>
@@ -22167,7 +22176,7 @@
         <v>0.57362817051024328</v>
       </c>
     </row>
-    <row r="444" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="444" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>544</v>
       </c>
@@ -22209,7 +22218,7 @@
         <v>1.1868773188982958E-3</v>
       </c>
     </row>
-    <row r="445" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="445" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>531</v>
       </c>
@@ -22251,7 +22260,7 @@
         <v>0.61419735888031768</v>
       </c>
     </row>
-    <row r="446" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="446" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>405</v>
       </c>
@@ -22331,7 +22340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="448" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="448" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>522</v>
       </c>
@@ -22373,7 +22382,7 @@
         <v>1.2738259040935463E-2</v>
       </c>
     </row>
-    <row r="449" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="449" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>312</v>
       </c>
@@ -22411,7 +22420,7 @@
         <v>5.7174924741473808E-2</v>
       </c>
     </row>
-    <row r="450" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="450" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>187</v>
       </c>
@@ -22453,7 +22462,7 @@
         <v>8.6179428414163875E-4</v>
       </c>
     </row>
-    <row r="451" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="451" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>257</v>
       </c>
@@ -22495,7 +22504,7 @@
         <v>0.49084730413962552</v>
       </c>
     </row>
-    <row r="452" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="452" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>506</v>
       </c>
@@ -22575,7 +22584,7 @@
         <v>0.91346112806797486</v>
       </c>
     </row>
-    <row r="454" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="454" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>142</v>
       </c>
@@ -22617,7 +22626,7 @@
         <v>0.79944700452672679</v>
       </c>
     </row>
-    <row r="455" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="455" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>141</v>
       </c>
@@ -22663,7 +22672,7 @@
         <v>39.976345950164863</v>
       </c>
     </row>
-    <row r="456" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="456" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>224</v>
       </c>
@@ -22705,7 +22714,7 @@
         <v>0.10023709482146938</v>
       </c>
     </row>
-    <row r="457" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="457" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>671</v>
       </c>
@@ -22747,7 +22756,7 @@
         <v>0.51878690842799557</v>
       </c>
     </row>
-    <row r="458" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="458" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>273</v>
       </c>
@@ -22785,7 +22794,7 @@
         <v>0.11358835175962652</v>
       </c>
     </row>
-    <row r="459" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="459" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>385</v>
       </c>
@@ -22869,7 +22878,7 @@
         <v>0.10972750859664102</v>
       </c>
     </row>
-    <row r="461" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="461" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>381</v>
       </c>
@@ -22949,7 +22958,7 @@
         <v>0.94925745313271737</v>
       </c>
     </row>
-    <row r="463" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="463" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>240</v>
       </c>
@@ -22991,7 +23000,7 @@
         <v>0.58773648211189755</v>
       </c>
     </row>
-    <row r="464" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>658</v>
       </c>
@@ -23037,7 +23046,7 @@
         <v>8.7613868027200592</v>
       </c>
     </row>
-    <row r="465" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="465" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>532</v>
       </c>
@@ -23079,7 +23088,7 @@
         <v>0.47856823020952399</v>
       </c>
     </row>
-    <row r="466" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="466" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>391</v>
       </c>
@@ -23121,7 +23130,7 @@
         <v>0.79129084148347406</v>
       </c>
     </row>
-    <row r="467" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="467" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>226</v>
       </c>
@@ -23197,7 +23206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="469" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="469" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>491</v>
       </c>
@@ -23239,7 +23248,7 @@
         <v>0.51483371780520271</v>
       </c>
     </row>
-    <row r="470" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>313</v>
       </c>
@@ -23323,7 +23332,7 @@
         <v>1.4838805411102286E-2</v>
       </c>
     </row>
-    <row r="472" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="472" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>143</v>
       </c>
@@ -23361,7 +23370,7 @@
         <v>7.449054386685032E-2</v>
       </c>
     </row>
-    <row r="473" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="473" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>432</v>
       </c>
@@ -23403,7 +23412,7 @@
         <v>0.69482844816632272</v>
       </c>
     </row>
-    <row r="474" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="474" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>617</v>
       </c>
@@ -23449,7 +23458,7 @@
         <v>7.6913202927470232</v>
       </c>
     </row>
-    <row r="475" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>388</v>
       </c>
@@ -23491,7 +23500,7 @@
         <v>0.88359236334864311</v>
       </c>
     </row>
-    <row r="476" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="476" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>535</v>
       </c>
@@ -23533,7 +23542,7 @@
         <v>0.40324571334082804</v>
       </c>
     </row>
-    <row r="477" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="477" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>228</v>
       </c>
@@ -23575,7 +23584,7 @@
         <v>0.93349344577351878</v>
       </c>
     </row>
-    <row r="478" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="478" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>166</v>
       </c>
@@ -23697,7 +23706,7 @@
         <v>0.96593008503263633</v>
       </c>
     </row>
-    <row r="481" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="481" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>184</v>
       </c>
@@ -23743,7 +23752,7 @@
         <v>6.2760666127308138</v>
       </c>
     </row>
-    <row r="482" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="482" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A482">
         <v>194</v>
       </c>
@@ -23899,7 +23908,7 @@
         <v>0.89973711717143745</v>
       </c>
     </row>
-    <row r="486" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="486" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A486">
         <v>524</v>
       </c>
@@ -23945,7 +23954,7 @@
         <v>21.458982648967076</v>
       </c>
     </row>
-    <row r="487" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="487" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A487">
         <v>223</v>
       </c>
@@ -23987,7 +23996,7 @@
         <v>0.91828669704948951</v>
       </c>
     </row>
-    <row r="488" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="488" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A488">
         <v>211</v>
       </c>
@@ -24029,7 +24038,7 @@
         <v>0.92119056280130795</v>
       </c>
     </row>
-    <row r="489" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="489" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A489">
         <v>266</v>
       </c>
@@ -24075,7 +24084,7 @@
         <v>8.3594662792323149</v>
       </c>
     </row>
-    <row r="490" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="490" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A490">
         <v>285</v>
       </c>
@@ -24117,7 +24126,7 @@
         <v>0.51199030166714321</v>
       </c>
     </row>
-    <row r="491" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="491" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A491">
         <v>418</v>
       </c>
@@ -24155,7 +24164,7 @@
         <v>0.29769736389405399</v>
       </c>
     </row>
-    <row r="492" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="492" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A492">
         <v>231</v>
       </c>
@@ -24231,7 +24240,7 @@
         <v>1.6336524452955442E-2</v>
       </c>
     </row>
-    <row r="494" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="494" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A494">
         <v>496</v>
       </c>
@@ -24273,7 +24282,7 @@
         <v>0.80329630500790261</v>
       </c>
     </row>
-    <row r="495" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="495" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A495">
         <v>673</v>
       </c>
@@ -24315,7 +24324,7 @@
         <v>0.82985112458871879</v>
       </c>
     </row>
-    <row r="496" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="496" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A496">
         <v>474</v>
       </c>
@@ -24395,7 +24404,7 @@
         <v>0.93964398208367084</v>
       </c>
     </row>
-    <row r="498" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="498" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A498">
         <v>384</v>
       </c>
@@ -24437,7 +24446,7 @@
         <v>0.87158705255410229</v>
       </c>
     </row>
-    <row r="499" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="499" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A499">
         <v>207</v>
       </c>
@@ -24479,7 +24488,7 @@
         <v>0.73389125639252806</v>
       </c>
     </row>
-    <row r="500" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="500" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A500">
         <v>161</v>
       </c>
@@ -24559,7 +24568,7 @@
         <v>0.72880812491086844</v>
       </c>
     </row>
-    <row r="502" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A502">
         <v>176</v>
       </c>
@@ -24723,7 +24732,7 @@
         <v>0.5623098124436503</v>
       </c>
     </row>
-    <row r="506" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="506" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A506">
         <v>665</v>
       </c>
@@ -24769,7 +24778,7 @@
         <v>17.561423765638917</v>
       </c>
     </row>
-    <row r="507" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="507" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A507">
         <v>279</v>
       </c>
@@ -24807,7 +24816,7 @@
         <v>0.28200243141148834</v>
       </c>
     </row>
-    <row r="508" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="508" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A508">
         <v>250</v>
       </c>
@@ -24853,7 +24862,7 @@
         <v>37.191619425242138</v>
       </c>
     </row>
-    <row r="509" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="509" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A509">
         <v>566</v>
       </c>
@@ -24933,7 +24942,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="511" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="511" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A511">
         <v>131</v>
       </c>
@@ -25051,7 +25060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="514" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="514" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A514">
         <v>170</v>
       </c>
@@ -25093,7 +25102,7 @@
         <v>0.57459081826297109</v>
       </c>
     </row>
-    <row r="515" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="515" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A515">
         <v>362</v>
       </c>
@@ -25173,7 +25182,7 @@
         <v>0.99651004209243921</v>
       </c>
     </row>
-    <row r="517" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="517" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A517">
         <v>690</v>
       </c>
@@ -25291,7 +25300,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="520" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="520" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A520">
         <v>452</v>
       </c>
@@ -25337,7 +25346,7 @@
         <v>21.470427244944176</v>
       </c>
     </row>
-    <row r="521" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="521" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A521">
         <v>395</v>
       </c>
@@ -25413,7 +25422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="523" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A523">
         <v>580</v>
       </c>
@@ -25493,7 +25502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="525" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A525">
         <v>526</v>
       </c>
@@ -25539,7 +25548,7 @@
         <v>44.923996664158132</v>
       </c>
     </row>
-    <row r="526" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="526" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A526">
         <v>156</v>
       </c>
@@ -25585,7 +25594,7 @@
         <v>20.659089442095432</v>
       </c>
     </row>
-    <row r="527" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A527">
         <v>188</v>
       </c>
@@ -25627,7 +25636,7 @@
         <v>0.11017044289965017</v>
       </c>
     </row>
-    <row r="528" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="528" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A528">
         <v>364</v>
       </c>
@@ -25669,7 +25678,7 @@
         <v>0.42058800524440898</v>
       </c>
     </row>
-    <row r="529" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="529" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A529">
         <v>517</v>
       </c>
@@ -25745,7 +25754,7 @@
         <v>0.99777672654608884</v>
       </c>
     </row>
-    <row r="531" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A531">
         <v>406</v>
       </c>
@@ -25791,7 +25800,7 @@
         <v>52.233618606651511</v>
       </c>
     </row>
-    <row r="532" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A532">
         <v>296</v>
       </c>
@@ -25829,7 +25838,7 @@
         <v>0.17439450194745751</v>
       </c>
     </row>
-    <row r="533" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A533">
         <v>683</v>
       </c>
@@ -25871,7 +25880,7 @@
         <v>1.7943977643498506E-3</v>
       </c>
     </row>
-    <row r="534" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A534">
         <v>473</v>
       </c>
@@ -25913,7 +25922,7 @@
         <v>8.624935530118169E-2</v>
       </c>
     </row>
-    <row r="535" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A535">
         <v>53</v>
       </c>
@@ -25951,7 +25960,7 @@
         <v>0.56061116714246817</v>
       </c>
     </row>
-    <row r="536" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="536" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A536">
         <v>453</v>
       </c>
@@ -25993,7 +26002,7 @@
         <v>0.5526131069924427</v>
       </c>
     </row>
-    <row r="537" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="537" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A537">
         <v>564</v>
       </c>
@@ -26035,7 +26044,7 @@
         <v>0.78648742090540968</v>
       </c>
     </row>
-    <row r="538" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="538" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A538">
         <v>607</v>
       </c>
@@ -26073,7 +26082,7 @@
         <v>0.76420878788111857</v>
       </c>
     </row>
-    <row r="539" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="539" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A539">
         <v>401</v>
       </c>
@@ -26115,7 +26124,7 @@
         <v>0.35864316218299869</v>
       </c>
     </row>
-    <row r="540" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="540" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A540">
         <v>256</v>
       </c>
@@ -26157,7 +26166,7 @@
         <v>3.4275020894503571E-3</v>
       </c>
     </row>
-    <row r="541" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A541">
         <v>208</v>
       </c>
@@ -26195,7 +26204,7 @@
         <v>0.42297586335729603</v>
       </c>
     </row>
-    <row r="542" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A542">
         <v>463</v>
       </c>
@@ -26279,7 +26288,7 @@
         <v>0.98260215311309307</v>
       </c>
     </row>
-    <row r="544" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A544">
         <v>99</v>
       </c>
@@ -26321,7 +26330,7 @@
         <v>0.25318637694973206</v>
       </c>
     </row>
-    <row r="545" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A545">
         <v>20</v>
       </c>
@@ -26405,7 +26414,7 @@
         <v>0.46643350765976599</v>
       </c>
     </row>
-    <row r="547" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A547">
         <v>291</v>
       </c>
@@ -26443,7 +26452,7 @@
         <v>0.16895907492389298</v>
       </c>
     </row>
-    <row r="548" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="548" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A548" s="11">
         <v>649</v>
       </c>
@@ -26485,7 +26494,7 @@
         <v>0.83507685909741292</v>
       </c>
     </row>
-    <row r="549" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="549" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A549">
         <v>495</v>
       </c>
@@ -26530,7 +26539,7 @@
         <v>1363</v>
       </c>
     </row>
-    <row r="550" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="550" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A550">
         <v>664</v>
       </c>
@@ -26682,7 +26691,7 @@
         <v>0.86400628187642847</v>
       </c>
     </row>
-    <row r="554" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A554">
         <v>500</v>
       </c>
@@ -26876,7 +26885,7 @@
         <v>0.6249702624920539</v>
       </c>
     </row>
-    <row r="559" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A559">
         <v>209</v>
       </c>
@@ -26918,7 +26927,7 @@
         <v>0.14269508860400854</v>
       </c>
     </row>
-    <row r="560" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A560">
         <v>55</v>
       </c>
@@ -26964,7 +26973,7 @@
         <v>33.029553398666188</v>
       </c>
     </row>
-    <row r="561" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="561" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A561">
         <v>688</v>
       </c>
@@ -27044,7 +27053,7 @@
         <v>1.7058863795674463E-3</v>
       </c>
     </row>
-    <row r="563" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="563" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A563">
         <v>122</v>
       </c>
@@ -27196,7 +27205,7 @@
         <v>0.10935852864760727</v>
       </c>
     </row>
-    <row r="567" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="567" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A567">
         <v>232</v>
       </c>
@@ -27234,7 +27243,7 @@
         <v>0.47494124432304297</v>
       </c>
     </row>
-    <row r="568" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="568" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A568">
         <v>369</v>
       </c>
@@ -27276,7 +27285,7 @@
         <v>0.25778739326096994</v>
       </c>
     </row>
-    <row r="569" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="569" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A569">
         <v>123</v>
       </c>
@@ -27314,7 +27323,7 @@
         <v>0.65067926915593577</v>
       </c>
     </row>
-    <row r="570" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="570" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A570">
         <v>436</v>
       </c>
@@ -27356,7 +27365,7 @@
         <v>0.19363689687095426</v>
       </c>
     </row>
-    <row r="571" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="571" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A571">
         <v>311</v>
       </c>
@@ -27398,7 +27407,7 @@
         <v>0.1918592395119198</v>
       </c>
     </row>
-    <row r="572" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="572" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A572">
         <v>518</v>
       </c>
@@ -27436,7 +27445,7 @@
         <v>0.9423942931654925</v>
       </c>
     </row>
-    <row r="573" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="573" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A573">
         <v>203</v>
       </c>
@@ -27520,7 +27529,7 @@
         <v>9.581221491129305E-4</v>
       </c>
     </row>
-    <row r="575" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="575" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A575">
         <v>280</v>
       </c>
@@ -27558,7 +27567,7 @@
         <v>0.47205806279816259</v>
       </c>
     </row>
-    <row r="576" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="576" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A576">
         <v>684</v>
       </c>
@@ -27638,7 +27647,7 @@
         <v>4.1996310287098652E-2</v>
       </c>
     </row>
-    <row r="578" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="578" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A578">
         <v>512</v>
       </c>
@@ -27684,7 +27693,7 @@
         <v>49.373695413078991</v>
       </c>
     </row>
-    <row r="579" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="579" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A579">
         <v>547</v>
       </c>
@@ -27726,7 +27735,7 @@
         <v>3.8545432943975416E-2</v>
       </c>
     </row>
-    <row r="580" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="580" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A580">
         <v>134</v>
       </c>
@@ -27764,7 +27773,7 @@
         <v>0.60359185638044965</v>
       </c>
     </row>
-    <row r="581" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="581" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A581">
         <v>368</v>
       </c>
@@ -27802,7 +27811,7 @@
         <v>0.93729695358015952</v>
       </c>
     </row>
-    <row r="582" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="582" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A582">
         <v>314</v>
       </c>
@@ -27840,7 +27849,7 @@
         <v>0.58825138277812528</v>
       </c>
     </row>
-    <row r="583" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="583" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A583">
         <v>538</v>
       </c>
@@ -27886,7 +27895,7 @@
         <v>65.490960638983992</v>
       </c>
     </row>
-    <row r="584" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="584" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A584">
         <v>271</v>
       </c>
@@ -27932,7 +27941,7 @@
         <v>50.416250218245757</v>
       </c>
     </row>
-    <row r="585" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="585" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A585">
         <v>556</v>
       </c>
@@ -27974,7 +27983,7 @@
         <v>0.1918123588150909</v>
       </c>
     </row>
-    <row r="586" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="586" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A586">
         <v>107</v>
       </c>
@@ -28012,7 +28021,7 @@
         <v>0.59162967835370517</v>
       </c>
     </row>
-    <row r="587" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="587" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A587">
         <v>152</v>
       </c>
@@ -28050,7 +28059,7 @@
         <v>0.47052437474608977</v>
       </c>
     </row>
-    <row r="588" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="588" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A588">
         <v>586</v>
       </c>
@@ -28092,7 +28101,7 @@
         <v>7.2936417419908336E-4</v>
       </c>
     </row>
-    <row r="589" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="589" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A589">
         <v>678</v>
       </c>
@@ -28252,7 +28261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="593" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="593" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A593">
         <v>661</v>
       </c>
@@ -28294,7 +28303,7 @@
         <v>3.1868120946644866E-2</v>
       </c>
     </row>
-    <row r="594" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A594">
         <v>67</v>
       </c>
@@ -28373,7 +28382,7 @@
         <v>8.5061352748685509E-2</v>
       </c>
     </row>
-    <row r="596" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="596" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A596">
         <v>119</v>
       </c>
@@ -28415,7 +28424,7 @@
         <v>0.1993913799784747</v>
       </c>
     </row>
-    <row r="597" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="597" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A597">
         <v>514</v>
       </c>
@@ -28537,7 +28546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="600" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="600" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A600">
         <v>460</v>
       </c>
@@ -28617,7 +28626,7 @@
         <v>0.13304528013843467</v>
       </c>
     </row>
-    <row r="602" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="602" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A602">
         <v>590</v>
       </c>
@@ -28663,7 +28672,7 @@
         <v>78.213474966654758</v>
       </c>
     </row>
-    <row r="603" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="603" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A603">
         <v>274</v>
       </c>
@@ -28705,7 +28714,7 @@
         <v>0.12981738490656985</v>
       </c>
     </row>
-    <row r="604" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="604" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A604">
         <v>178</v>
       </c>
@@ -28781,7 +28790,7 @@
         <v>0.57974155553927709</v>
       </c>
     </row>
-    <row r="606" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="606" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A606">
         <v>179</v>
       </c>
@@ -28827,7 +28836,7 @@
         <v>171.8542715370894</v>
       </c>
     </row>
-    <row r="607" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="607" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A607">
         <v>342</v>
       </c>
@@ -28865,7 +28874,7 @@
         <v>0.99620714163683921</v>
       </c>
     </row>
-    <row r="608" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="608" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A608">
         <v>181</v>
       </c>
@@ -28907,7 +28916,7 @@
         <v>0.64442580672409699</v>
       </c>
     </row>
-    <row r="609" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="609" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A609">
         <v>217</v>
       </c>
@@ -28945,7 +28954,7 @@
         <v>0.28630799076230928</v>
       </c>
     </row>
-    <row r="610" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="610" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A610">
         <v>663</v>
       </c>
@@ -28987,7 +28996,7 @@
         <v>0.34200398523918352</v>
       </c>
     </row>
-    <row r="611" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="611" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A611">
         <v>583</v>
       </c>
@@ -29029,7 +29038,7 @@
         <v>0.27282367565517462</v>
       </c>
     </row>
-    <row r="612" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="612" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A612">
         <v>615</v>
       </c>
@@ -29075,7 +29084,7 @@
         <v>75.835606938632608</v>
       </c>
     </row>
-    <row r="613" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="613" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A613">
         <v>350</v>
       </c>
@@ -29117,7 +29126,7 @@
         <v>0.61926744130916678</v>
       </c>
     </row>
-    <row r="614" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="614" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A614">
         <v>600</v>
       </c>
@@ -29155,7 +29164,7 @@
         <v>0.8799171082835785</v>
       </c>
     </row>
-    <row r="615" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="615" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A615">
         <v>344</v>
       </c>
@@ -29277,7 +29286,7 @@
         <v>0.24020258968424646</v>
       </c>
     </row>
-    <row r="618" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="618" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A618">
         <v>191</v>
       </c>
@@ -29315,7 +29324,7 @@
         <v>0.11053498117292319</v>
       </c>
     </row>
-    <row r="619" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="619" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A619">
         <v>189</v>
       </c>
@@ -29357,7 +29366,7 @@
         <v>4.6314768153347341E-2</v>
       </c>
     </row>
-    <row r="620" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="620" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A620">
         <v>628</v>
       </c>
@@ -29471,7 +29480,7 @@
         <v>0.57678762466243116</v>
       </c>
     </row>
-    <row r="623" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="623" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A623">
         <v>245</v>
       </c>
@@ -29513,7 +29522,7 @@
       </c>
       <c r="N623" s="15"/>
     </row>
-    <row r="624" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="624" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A624">
         <v>10</v>
       </c>
@@ -29589,7 +29598,7 @@
         <v>0.14931262940434331</v>
       </c>
     </row>
-    <row r="626" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="626" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A626">
         <v>636</v>
       </c>
@@ -29627,7 +29636,7 @@
         <v>0.58875385662980084</v>
       </c>
     </row>
-    <row r="627" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="627" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A627">
         <v>309</v>
       </c>
@@ -29665,7 +29674,7 @@
         <v>0.78666799960329659</v>
       </c>
     </row>
-    <row r="628" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="628" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A628">
         <v>427</v>
       </c>
@@ -29745,7 +29754,7 @@
         <v>0.34416650317322528</v>
       </c>
     </row>
-    <row r="630" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="630" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A630">
         <v>565</v>
       </c>
@@ -29787,7 +29796,7 @@
         <v>0.52369855240158247</v>
       </c>
     </row>
-    <row r="631" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="631" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A631">
         <v>101</v>
       </c>
@@ -29825,7 +29834,7 @@
         <v>0.57026205361840854</v>
       </c>
     </row>
-    <row r="632" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="632" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A632">
         <v>87</v>
       </c>
@@ -29863,7 +29872,7 @@
         <v>0.84024159988861014</v>
       </c>
     </row>
-    <row r="633" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="633" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A633">
         <v>118</v>
       </c>
@@ -29905,7 +29914,7 @@
         <v>0.10792532533942323</v>
       </c>
     </row>
-    <row r="634" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="634" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A634">
         <v>65</v>
       </c>
@@ -29981,7 +29990,7 @@
         <v>0.51042503683879281</v>
       </c>
     </row>
-    <row r="636" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="636" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A636">
         <v>108</v>
       </c>
@@ -30019,7 +30028,7 @@
         <v>0.73704919667455004</v>
       </c>
     </row>
-    <row r="637" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="637" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A637">
         <v>127</v>
       </c>
@@ -30099,7 +30108,7 @@
         <v>0.76692261621462288</v>
       </c>
     </row>
-    <row r="639" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="639" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A639">
         <v>537</v>
       </c>
@@ -30179,7 +30188,7 @@
         <v>7.1661429170581617E-2</v>
       </c>
     </row>
-    <row r="641" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="641" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A641">
         <v>173</v>
       </c>
@@ -30217,7 +30226,7 @@
         <v>0.89590487670442398</v>
       </c>
     </row>
-    <row r="642" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="642" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A642">
         <v>470</v>
       </c>
@@ -30297,7 +30306,7 @@
         <v>1.4518078249672071E-2</v>
       </c>
     </row>
-    <row r="644" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="644" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A644">
         <v>610</v>
       </c>
@@ -30343,7 +30352,7 @@
         <v>70.047023040388552</v>
       </c>
     </row>
-    <row r="645" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="645" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A645">
         <v>449</v>
       </c>
@@ -30499,7 +30508,7 @@
         <v>0.52142868680292254</v>
       </c>
     </row>
-    <row r="649" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="649" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A649">
         <v>346</v>
       </c>
@@ -30617,7 +30626,7 @@
         <v>0.17902458833350809</v>
       </c>
     </row>
-    <row r="652" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="652" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A652">
         <v>497</v>
       </c>
@@ -30655,7 +30664,7 @@
         <v>0.99402401537256024</v>
       </c>
     </row>
-    <row r="653" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="653" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A653">
         <v>5</v>
       </c>
@@ -30697,7 +30706,7 @@
         <v>0.7827562702254196</v>
       </c>
     </row>
-    <row r="654" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="654" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A654">
         <v>653</v>
       </c>
@@ -30777,7 +30786,7 @@
         <v>0.40866712122846222</v>
       </c>
     </row>
-    <row r="656" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="656" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A656">
         <v>347</v>
       </c>
@@ -30823,7 +30832,7 @@
         <v>153.9440241162215</v>
       </c>
     </row>
-    <row r="657" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="657" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A657">
         <v>132</v>
       </c>
@@ -30861,7 +30870,7 @@
         <v>0.96981751032707553</v>
       </c>
     </row>
-    <row r="658" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="658" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A658">
         <v>448</v>
       </c>
@@ -30899,7 +30908,7 @@
         <v>0.89953684576787896</v>
       </c>
     </row>
-    <row r="659" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="659" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A659">
         <v>62</v>
       </c>
@@ -30937,7 +30946,7 @@
         <v>0.13132264335966012</v>
       </c>
     </row>
-    <row r="660" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="660" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A660">
         <v>34</v>
       </c>
@@ -30975,7 +30984,7 @@
         <v>9.9324264051517175E-2</v>
       </c>
     </row>
-    <row r="661" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="661" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A661">
         <v>32</v>
       </c>
@@ -31051,7 +31060,7 @@
         <v>0.9851177322713689</v>
       </c>
     </row>
-    <row r="663" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="663" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A663">
         <v>629</v>
       </c>
@@ -31093,7 +31102,7 @@
         <v>0.22221080553086198</v>
       </c>
     </row>
-    <row r="664" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="664" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A664">
         <v>511</v>
       </c>
@@ -31177,7 +31186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="666" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="666" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A666">
         <v>70</v>
       </c>
@@ -31223,7 +31232,7 @@
         <v>146.80360149525657</v>
       </c>
     </row>
-    <row r="667" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="667" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A667">
         <v>691</v>
       </c>
@@ -31265,7 +31274,7 @@
         <v>0.40654267133671118</v>
       </c>
     </row>
-    <row r="668" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A668">
         <v>677</v>
       </c>
@@ -31307,7 +31316,7 @@
         <v>0.20526548811090656</v>
       </c>
     </row>
-    <row r="669" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="669" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A669">
         <v>508</v>
       </c>
@@ -31391,7 +31400,7 @@
         <v>8.7202770282953906E-3</v>
       </c>
     </row>
-    <row r="671" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="671" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A671">
         <v>642</v>
       </c>
@@ -31433,7 +31442,7 @@
         <v>0.13343121862756985</v>
       </c>
     </row>
-    <row r="672" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="672" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A672">
         <v>64</v>
       </c>
@@ -31512,7 +31521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="674" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="674" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A674">
         <v>139</v>
       </c>
@@ -31558,7 +31567,7 @@
         <v>159.48795159217983</v>
       </c>
     </row>
-    <row r="675" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="675" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A675">
         <v>100</v>
       </c>
@@ -31604,7 +31613,7 @@
         <v>145.17588584770996</v>
       </c>
     </row>
-    <row r="676" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="676" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A676">
         <v>612</v>
       </c>
@@ -31650,7 +31659,7 @@
         <v>86.788236862928926</v>
       </c>
     </row>
-    <row r="677" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="677" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A677">
         <v>96</v>
       </c>
@@ -31726,7 +31735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="679" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="679" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A679">
         <v>467</v>
       </c>
@@ -31768,7 +31777,7 @@
         <v>0.31243637805991009</v>
       </c>
     </row>
-    <row r="680" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="680" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A680">
         <v>422</v>
       </c>
@@ -31806,7 +31815,7 @@
         <v>0.78572932667234407</v>
       </c>
     </row>
-    <row r="681" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="681" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A681">
         <v>569</v>
       </c>
@@ -32000,7 +32009,7 @@
         <v>0.99419746197421666</v>
       </c>
     </row>
-    <row r="686" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="686" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A686">
         <v>414</v>
       </c>
@@ -32038,7 +32047,7 @@
         <v>0.93985691504823321</v>
       </c>
     </row>
-    <row r="687" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="687" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A687">
         <v>428</v>
       </c>
@@ -32156,7 +32165,7 @@
         <v>6.9010310254079992E-4</v>
       </c>
     </row>
-    <row r="690" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="690" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A690">
         <v>227</v>
       </c>
@@ -32198,7 +32207,7 @@
         <v>9.276065469379419E-3</v>
       </c>
     </row>
-    <row r="691" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="691" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A691">
         <v>22</v>
       </c>
@@ -32274,7 +32283,7 @@
         <v>0.84603792825921187</v>
       </c>
     </row>
-    <row r="693" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="693" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A693">
         <v>317</v>
       </c>
@@ -32316,7 +32325,7 @@
         <v>1.0456632089220817E-2</v>
       </c>
     </row>
-    <row r="694" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="694" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A694">
         <v>438</v>
       </c>
@@ -32392,7 +32401,7 @@
         <v>0.68063931494108576</v>
       </c>
     </row>
-    <row r="696" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="696" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A696">
         <v>1</v>
       </c>
@@ -33178,7 +33187,7 @@
         <v>0.98988221297852264</v>
       </c>
     </row>
-    <row r="718" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="718" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A718">
         <v>175</v>
       </c>
@@ -33220,7 +33229,7 @@
         <v>2.3199950611834261E-2</v>
       </c>
     </row>
-    <row r="719" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="719" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A719">
         <v>355</v>
       </c>
@@ -33752,7 +33761,7 @@
         <v>0.57184201222057018</v>
       </c>
     </row>
-    <row r="734" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="734" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A734">
         <v>177</v>
       </c>
@@ -33969,7 +33978,7 @@
         <v>0.6729763137966116</v>
       </c>
     </row>
-    <row r="740" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="740" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A740">
         <v>335</v>
       </c>
@@ -38071,7 +38080,7 @@
         <v>0.91810242846180479</v>
       </c>
     </row>
-    <row r="857" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="857" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A857">
         <v>307</v>
       </c>
@@ -39093,7 +39102,7 @@
         <v>0.69887847405066672</v>
       </c>
     </row>
-    <row r="886" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="886" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A886">
         <v>286</v>
       </c>
@@ -39520,7 +39529,7 @@
         <v>0.52307758073688215</v>
       </c>
     </row>
-    <row r="898" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="898" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A898">
         <v>623</v>
       </c>
@@ -41627,7 +41636,7 @@
         <v>0.47891570190293131</v>
       </c>
     </row>
-    <row r="958" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="958" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A958">
         <v>578</v>
       </c>
@@ -41949,7 +41958,7 @@
         <v>0.84634258296711729</v>
       </c>
     </row>
-    <row r="967" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="967" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A967">
         <v>597</v>
       </c>
@@ -42341,7 +42350,7 @@
         <v>0.99201683592585976</v>
       </c>
     </row>
-    <row r="978" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="978" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A978">
         <v>503</v>
       </c>
@@ -43258,7 +43267,7 @@
         <v>5.6078682211608E-2</v>
       </c>
     </row>
-    <row r="1004" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1004" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1004">
         <v>358</v>
       </c>
@@ -46275,7 +46284,7 @@
         <v>0.93446797948681537</v>
       </c>
     </row>
-    <row r="1090" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1090" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1090">
         <v>11</v>
       </c>
@@ -48627,7 +48636,7 @@
         <v>4.6523373361543226E-2</v>
       </c>
     </row>
-    <row r="1157" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1157" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1157">
         <v>220</v>
       </c>
@@ -48750,7 +48759,7 @@
         <v>158.58128221564721</v>
       </c>
     </row>
-    <row r="1160" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1160" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1160">
         <v>345</v>
       </c>
@@ -50118,7 +50127,7 @@
         <v>0.95726769219762475</v>
       </c>
     </row>
-    <row r="1199" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1199" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1199">
         <v>193</v>
       </c>
@@ -50689,7 +50698,7 @@
         <v>0.94895879132744443</v>
       </c>
     </row>
-    <row r="1215" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1215" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1215">
         <v>455</v>
       </c>
@@ -51050,7 +51059,7 @@
         <v>0.99616985471171748</v>
       </c>
     </row>
-    <row r="1225" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1225" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1225">
         <v>244</v>
       </c>
@@ -51687,7 +51696,7 @@
         <v>0.99681510949395535</v>
       </c>
     </row>
-    <row r="1243" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1243" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1243">
         <v>154</v>
       </c>
@@ -52674,7 +52683,7 @@
         <v>7.2789669587380234E-3</v>
       </c>
     </row>
-    <row r="1271" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1271" spans="1:13" hidden="1" x14ac:dyDescent="0.25">
       <c r="A1271">
         <v>492</v>
       </c>
@@ -64294,6 +64303,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A4:L1279">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="16"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="5">
       <filters>
         <filter val="1"/>
@@ -64314,10 +64328,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:R20"/>
+  <dimension ref="B2:T21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T20" sqref="T20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64325,9 +64339,10 @@
     <col min="7" max="7" width="12.42578125" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="1.85546875" customWidth="1"/>
+    <col min="15" max="15" width="1.85546875" customWidth="1"/>
+    <col min="16" max="16" width="17" customWidth="1"/>
     <col min="17" max="17" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.25">
@@ -64395,6 +64410,10 @@
       <c r="L5" s="21"/>
       <c r="M5" s="21"/>
       <c r="N5" s="21"/>
+      <c r="P5">
+        <f>B5</f>
+        <v>1</v>
+      </c>
       <c r="Q5" s="7">
         <v>24283</v>
       </c>
@@ -64437,6 +64456,10 @@
       <c r="N6" s="25">
         <v>0.3535892056968914</v>
       </c>
+      <c r="P6">
+        <f t="shared" ref="P6:P20" si="0">B6</f>
+        <v>2</v>
+      </c>
       <c r="Q6" s="24">
         <v>232.13</v>
       </c>
@@ -64482,7 +64505,10 @@
       <c r="O7" s="21" t="s">
         <v>1353</v>
       </c>
-      <c r="P7" s="21"/>
+      <c r="P7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="Q7" s="7">
         <v>23230</v>
       </c>
@@ -64524,6 +64550,10 @@
       </c>
       <c r="N8" s="25">
         <v>0.20471301274093254</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="Q8" s="24">
         <v>932.06</v>
@@ -64545,6 +64575,10 @@
       <c r="L9" s="21"/>
       <c r="M9" s="21"/>
       <c r="N9" s="21"/>
+      <c r="P9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="Q9" s="7">
         <v>23273</v>
       </c>
@@ -64589,6 +64623,10 @@
       <c r="N10" s="24">
         <v>0</v>
       </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="21">
@@ -64630,6 +64668,10 @@
       <c r="N11" s="25">
         <v>9.9324264051517175E-2</v>
       </c>
+      <c r="P11">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
       <c r="Q11" s="13">
         <v>531.42999999999995</v>
       </c>
@@ -64680,7 +64722,10 @@
       <c r="O12" s="21" t="s">
         <v>1360</v>
       </c>
-      <c r="P12" s="21"/>
+      <c r="P12">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
       <c r="Q12" s="24">
         <v>931.84</v>
       </c>
@@ -64726,7 +64771,10 @@
         <v>4.150370709983444E-2</v>
       </c>
       <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
+      <c r="P13">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="Q13" s="7">
         <v>23174</v>
       </c>
@@ -64773,6 +64821,10 @@
       </c>
       <c r="O14" t="s">
         <v>1353</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.25">
@@ -64791,6 +64843,10 @@
       <c r="L15" s="21"/>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
       <c r="Q15" s="7">
         <v>24216</v>
       </c>
@@ -64836,11 +64892,15 @@
       <c r="O16" s="21" t="s">
         <v>1362</v>
       </c>
+      <c r="P16">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
       <c r="Q16" s="28">
         <v>232.85</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="7">
         <v>13</v>
       </c>
@@ -64881,8 +64941,12 @@
       <c r="O17" t="s">
         <v>1353</v>
       </c>
-    </row>
-    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="P17">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" s="7">
         <v>14</v>
       </c>
@@ -64922,8 +64986,12 @@
       <c r="N18" s="24">
         <v>0.59715159187267175</v>
       </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="P18">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" s="21">
         <v>15</v>
       </c>
@@ -64964,11 +65032,21 @@
         <v>0.75357775375040204</v>
       </c>
       <c r="O19" s="8"/>
+      <c r="P19">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
       <c r="Q19" s="24">
         <v>931.38</v>
       </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S19" t="s">
+        <v>1372</v>
+      </c>
+      <c r="T19" t="s">
+        <v>1373</v>
+      </c>
+    </row>
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B20" s="21">
         <v>16</v>
       </c>
@@ -65011,11 +65089,26 @@
       <c r="O20" s="25" t="s">
         <v>1368</v>
       </c>
+      <c r="P20">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
       <c r="Q20" s="13">
         <v>231.31</v>
       </c>
-      <c r="R20" s="24">
+      <c r="R20" s="13">
         <v>231.79</v>
+      </c>
+      <c r="S20" s="7">
+        <v>23161</v>
+      </c>
+      <c r="T20" s="7">
+        <v>23157</v>
+      </c>
+    </row>
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="R21" t="s">
+        <v>1371</v>
       </c>
     </row>
   </sheetData>

</xml_diff>